<commit_message>
Add new supplier page updated
</commit_message>
<xml_diff>
--- a/aturian-automation/src/test/resources/TestData/TestData.xlsx
+++ b/aturian-automation/src/test/resources/TestData/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
   <si>
     <t>Email</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>Automation Billing Notes123!@#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>Automation Deal</t>
   </si>
 </sst>
 </file>
@@ -609,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,6 +753,9 @@
       </c>
       <c r="P2" t="s">
         <v>67</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>85</v>
       </c>
       <c r="R2" t="s">
         <v>63</v>

</xml_diff>